<commit_message>
Treinamento FHIR & ajuste templates
</commit_message>
<xml_diff>
--- a/Entregaveis/Templates/Template mapeamento/Template mapeamento.xlsx
+++ b/Entregaveis/Templates/Template mapeamento/Template mapeamento.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moaassis\Documents\GitHub\HSL-IPS\Entregaveis\Templates\Template mapeamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/HSL-IPS-1/Entregaveis/Templates/Template mapeamento/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAF94A0-5F15-634A-8EB2-CD11C3847CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29140" windowHeight="15460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapeamento" sheetId="1" r:id="rId1"/>
-    <sheet name="Opções" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapeamento 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Equivalências" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapeamento 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapeamento!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="0">Mapeamento!$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mapeamento 1'!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">'Mapeamento 1'!$G$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -85,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,7 +178,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,25 +468,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="3" width="31.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -496,7 +498,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -508,7 +510,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -535,13 +537,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H3"/>
+  <autoFilter ref="A3:H3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"1..1,1..*,*..1,*..*"</formula1>
     </dataValidation>
   </dataValidations>
@@ -550,15 +552,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>Opções!$A$1:$G$1</xm:f>
+            <xm:f>Equivalências!$A$1:$G$1</xm:f>
           </x14:formula1>
           <xm:sqref>G4:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>'C:\Users\moaassis\Documents\HSL-IPS\Entregaveis\Mapeamentos\Templates\ConceptMap\BRImunobiológico\[Mapping BRImunobiológico.xlsx]Opções'!#REF!</xm:f>
+            <xm:f>'/Users/beatrizdefarialeao/Library/Containers/com.microsoft.Excel/Data/Documents/C:\Users\moaassis\Documents\HSL-IPS\Entregaveis\Mapeamentos\Templates\ConceptMap\BRImunobiológico\[Mapping BRImunobiológico.xlsx]Opções'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G3</xm:sqref>
         </x14:dataValidation>
@@ -569,19 +571,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -604,4 +606,16 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23BAC6EA-31E2-9142-A9C7-C165B6AC70B3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>